<commit_message>
forest rothc run and ready
</commit_message>
<xml_diff>
--- a/data/forest/forest_residues_IPCC.xlsx
+++ b/data/forest/forest_residues_IPCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/forest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_28030BAB286704F8B55CCBCBEFAD6F8E463B3ABF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE6BEB3F-87D4-4D58-BD4B-CEEDD44E702A}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_28030BAB286704F8B55CCBCBEFAD6F8E463B3ABF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69431A26-ECB3-4004-A48F-5CF67A1A47C4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,13 +753,13 @@
         <v>2</v>
       </c>
       <c r="F8" s="6">
-        <v>4.0999999999999996</v>
+        <v>1.6810069359086786</v>
       </c>
       <c r="G8" s="4">
         <v>3</v>
       </c>
       <c r="H8" s="6">
-        <v>4.0999999999999996</v>
+        <v>7.7631903477398474</v>
       </c>
       <c r="I8" s="4">
         <v>20</v>
@@ -785,13 +785,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="6">
-        <v>5.2</v>
+        <v>2.1320087967622268</v>
       </c>
       <c r="G9" s="4">
         <v>3</v>
       </c>
       <c r="H9" s="6">
-        <v>5.2</v>
+        <v>9.8459975142066369</v>
       </c>
       <c r="I9" s="4">
         <v>20</v>

</xml_diff>